<commit_message>
removed summary, added economics tracker
</commit_message>
<xml_diff>
--- a/Document_Processing_Pipeline_Steps.xlsx
+++ b/Document_Processing_Pipeline_Steps.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\DocProcessing\zealits\onpremdoc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96A7EF12-B346-4FF0-8841-E2E609F3400B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F46DEBBD-2EAD-411B-BE37-EAD0EFA0F742}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Pipeline Steps" sheetId="1" r:id="rId1"/>
-    <sheet name="Combined Steps" sheetId="2" r:id="rId2"/>
+    <sheet name="Short" sheetId="2" r:id="rId1"/>
+    <sheet name="Detail" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -1421,6 +1421,449 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:J13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8" customWidth="1"/>
+    <col min="2" max="2" width="25" customWidth="1"/>
+    <col min="3" max="3" width="50" customWidth="1"/>
+    <col min="4" max="4" width="20" customWidth="1"/>
+    <col min="5" max="5" width="35" customWidth="1"/>
+    <col min="6" max="6" width="40" customWidth="1"/>
+    <col min="7" max="7" width="30" customWidth="1"/>
+    <col min="8" max="8" width="25" customWidth="1"/>
+    <col min="9" max="9" width="30" customWidth="1"/>
+    <col min="10" max="10" width="38.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="90" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="6">
+        <v>1</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>243</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>244</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>247</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>248</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="90" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="6">
+        <v>2</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>250</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>251</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>252</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>253</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>254</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>255</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="90" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="6">
+        <v>3</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>257</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>258</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>259</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>260</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>262</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>263</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="90" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="6">
+        <v>4</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>265</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>266</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>267</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>268</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>269</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>270</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>271</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="90" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>273</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>274</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>275</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>276</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>277</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>278</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>279</v>
+      </c>
+      <c r="J6" s="5" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="90" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="6">
+        <v>6</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>281</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>282</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>283</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>284</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>285</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>286</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>287</v>
+      </c>
+      <c r="J7" s="5" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="90" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="6">
+        <v>7</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>289</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>290</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>291</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>292</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="J8" s="5" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="90" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="6">
+        <v>8</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>293</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>294</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>295</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>296</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>297</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="I9" s="5" t="s">
+        <v>298</v>
+      </c>
+      <c r="J9" s="5" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="90" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="6">
+        <v>9</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>300</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>301</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>302</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>303</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>304</v>
+      </c>
+      <c r="H10" s="5" t="s">
+        <v>305</v>
+      </c>
+      <c r="I10" s="5" t="s">
+        <v>306</v>
+      </c>
+      <c r="J10" s="5" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="90" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="6">
+        <v>10</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>308</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>309</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>310</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>311</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>312</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>313</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>314</v>
+      </c>
+      <c r="J11" s="5" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="90" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="6">
+        <v>11</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>316</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>317</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>318</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>319</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>320</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>321</v>
+      </c>
+      <c r="H12" s="5" t="s">
+        <v>322</v>
+      </c>
+      <c r="I12" s="5" t="s">
+        <v>323</v>
+      </c>
+      <c r="J12" s="5" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="90" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="6">
+        <v>12</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>234</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>325</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>326</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>240</v>
+      </c>
+      <c r="I13" s="5" t="s">
+        <v>327</v>
+      </c>
+      <c r="J13" s="5" t="s">
+        <v>328</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J31"/>
   <sheetViews>
@@ -2438,447 +2881,4 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:J13"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="8" customWidth="1"/>
-    <col min="2" max="2" width="25" customWidth="1"/>
-    <col min="3" max="3" width="50" customWidth="1"/>
-    <col min="4" max="4" width="20" customWidth="1"/>
-    <col min="5" max="5" width="35" customWidth="1"/>
-    <col min="6" max="6" width="40" customWidth="1"/>
-    <col min="7" max="7" width="30" customWidth="1"/>
-    <col min="8" max="8" width="25" customWidth="1"/>
-    <col min="9" max="9" width="30" customWidth="1"/>
-    <col min="10" max="10" width="38.28515625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="6">
-        <v>1</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>243</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>244</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>245</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>246</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>247</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="I2" s="5" t="s">
-        <v>248</v>
-      </c>
-      <c r="J2" s="5" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="6">
-        <v>2</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>250</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>251</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>252</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>253</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>254</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="I3" s="5" t="s">
-        <v>255</v>
-      </c>
-      <c r="J3" s="5" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="6">
-        <v>3</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>257</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>258</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>259</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>260</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>261</v>
-      </c>
-      <c r="H4" s="5" t="s">
-        <v>262</v>
-      </c>
-      <c r="I4" s="5" t="s">
-        <v>263</v>
-      </c>
-      <c r="J4" s="5" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="6">
-        <v>4</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>265</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>266</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>267</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>268</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>269</v>
-      </c>
-      <c r="H5" s="5" t="s">
-        <v>270</v>
-      </c>
-      <c r="I5" s="5" t="s">
-        <v>271</v>
-      </c>
-      <c r="J5" s="5" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="6">
-        <v>5</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>273</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>274</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>275</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>276</v>
-      </c>
-      <c r="G6" s="5" t="s">
-        <v>277</v>
-      </c>
-      <c r="H6" s="5" t="s">
-        <v>278</v>
-      </c>
-      <c r="I6" s="5" t="s">
-        <v>279</v>
-      </c>
-      <c r="J6" s="5" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="6">
-        <v>6</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>281</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>282</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>283</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>284</v>
-      </c>
-      <c r="G7" s="5" t="s">
-        <v>285</v>
-      </c>
-      <c r="H7" s="5" t="s">
-        <v>286</v>
-      </c>
-      <c r="I7" s="5" t="s">
-        <v>287</v>
-      </c>
-      <c r="J7" s="5" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="6">
-        <v>7</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>289</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>290</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>153</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>291</v>
-      </c>
-      <c r="G8" s="5" t="s">
-        <v>292</v>
-      </c>
-      <c r="H8" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="I8" s="5" t="s">
-        <v>157</v>
-      </c>
-      <c r="J8" s="5" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="6">
-        <v>8</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>293</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>294</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>168</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>295</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>296</v>
-      </c>
-      <c r="G9" s="5" t="s">
-        <v>297</v>
-      </c>
-      <c r="H9" s="5" t="s">
-        <v>163</v>
-      </c>
-      <c r="I9" s="5" t="s">
-        <v>298</v>
-      </c>
-      <c r="J9" s="5" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="6">
-        <v>9</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>300</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>301</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>176</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>302</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>303</v>
-      </c>
-      <c r="G10" s="5" t="s">
-        <v>304</v>
-      </c>
-      <c r="H10" s="5" t="s">
-        <v>305</v>
-      </c>
-      <c r="I10" s="5" t="s">
-        <v>306</v>
-      </c>
-      <c r="J10" s="5" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="6">
-        <v>10</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>308</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>309</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>176</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>310</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>311</v>
-      </c>
-      <c r="G11" s="5" t="s">
-        <v>312</v>
-      </c>
-      <c r="H11" s="5" t="s">
-        <v>313</v>
-      </c>
-      <c r="I11" s="5" t="s">
-        <v>314</v>
-      </c>
-      <c r="J11" s="5" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="6">
-        <v>11</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>316</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>317</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>318</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>319</v>
-      </c>
-      <c r="F12" s="5" t="s">
-        <v>320</v>
-      </c>
-      <c r="G12" s="5" t="s">
-        <v>321</v>
-      </c>
-      <c r="H12" s="5" t="s">
-        <v>322</v>
-      </c>
-      <c r="I12" s="5" t="s">
-        <v>323</v>
-      </c>
-      <c r="J12" s="5" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="6">
-        <v>12</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>234</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>325</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>236</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>237</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>326</v>
-      </c>
-      <c r="G13" s="5" t="s">
-        <v>239</v>
-      </c>
-      <c r="H13" s="5" t="s">
-        <v>240</v>
-      </c>
-      <c r="I13" s="5" t="s">
-        <v>327</v>
-      </c>
-      <c r="J13" s="5" t="s">
-        <v>328</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
 </file>
</xml_diff>